<commit_message>
commit on 'import and save'
</commit_message>
<xml_diff>
--- a/api/assets/resource/RestaurnatTemplate.xlsx
+++ b/api/assets/resource/RestaurnatTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Node\food-ordering-web\api\assets\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9E7D21-1DC7-45F9-9194-55E1D6DBE585}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CEDCD2-1762-4A24-BC66-57443597FDFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DF363CBE-6587-4F6F-AFC0-839F3ECBE201}"/>
   </bookViews>
@@ -33,19 +33,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Restaurnat Name</t>
+    <t>name</t>
   </si>
   <si>
-    <t>Email</t>
+    <t>email</t>
   </si>
   <si>
-    <t>Mobile</t>
+    <t>password</t>
   </si>
   <si>
-    <t>Address</t>
+    <t>mobile</t>
   </si>
   <si>
-    <t>Password</t>
+    <t>address</t>
   </si>
 </sst>
 </file>
@@ -400,12 +400,12 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
@@ -419,13 +419,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>